<commit_message>
Improved optimization, now we have no errors in the editor. And also nothing is draggable.
</commit_message>
<xml_diff>
--- a/excell/32.xlsx
+++ b/excell/32.xlsx
@@ -38,6 +38,9 @@
 22 Янв.</t>
   </si>
   <si>
+    <t>Физика (ЮН)</t>
+  </si>
+  <si>
     <t>Химия (G1234re213)</t>
   </si>
   <si>
@@ -51,9 +54,6 @@
   </si>
   <si>
     <t>Физика (Гриц)</t>
-  </si>
-  <si>
-    <t>Физика (ЮН)</t>
   </si>
   <si>
     <t>Понедельн.
@@ -473,61 +473,73 @@
         <v>5</v>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="2" spans="1:8">
+    <row customHeight="1" ht="18" r="2" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="27" r="3" spans="1:8">
+    </row>
+    <row r="3" spans="1:8">
       <c r="B3" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="18" r="4" spans="1:8">
+    </row>
+    <row customHeight="1" ht="30" r="4" spans="1:8">
       <c r="B4" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="27" r="5" spans="1:8">
       <c r="B5" s="3" t="n">
         <v>4</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row customHeight="1" ht="27" r="6" spans="1:8">
       <c r="B6" s="3" t="n">
         <v>5</v>
       </c>
+      <c r="C6" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="D6" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>9</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="22" r="7" spans="1:8">
       <c r="B7" s="3" t="n">
         <v>6</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -541,35 +553,56 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row customHeight="1" ht="27" r="10" spans="1:8">
       <c r="B10" s="3" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row customHeight="1" ht="27" r="11" spans="1:8">
+      <c r="D10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="18" r="11" spans="1:8">
       <c r="B11" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>8</v>
+      <c r="C11" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row customHeight="1" ht="27" r="12" spans="1:8">
       <c r="B12" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="E12" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="F12" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>9</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="27" r="13" spans="1:8">
       <c r="B13" s="3" t="n">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="G13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="27" r="14" spans="1:8">
       <c r="B14" s="3" t="n">
         <v>6</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -583,23 +616,20 @@
         <v>1</v>
       </c>
     </row>
-    <row customHeight="1" ht="27" r="17" spans="1:8">
+    <row customHeight="1" ht="23" r="17" spans="1:8">
       <c r="B17" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="27" r="18" spans="1:8">
+      <c r="E17" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="22" r="18" spans="1:8">
       <c r="B18" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="F18" s="4" t="s">
-        <v>8</v>
+      <c r="H18" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -664,9 +694,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row customHeight="1" ht="27" r="31" spans="1:8">
       <c r="B31" s="3" t="n">
         <v>2</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:8">

</xml_diff>

<commit_message>
Fixed saving to excell
</commit_message>
<xml_diff>
--- a/excell/32.xlsx
+++ b/excell/32.xlsx
@@ -14,7 +14,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+  <si>
+    <t>Расписание на 20 Мар. - 25 Мар.</t>
+  </si>
+  <si>
+    <t>6E</t>
+  </si>
+  <si>
+    <t>7E</t>
+  </si>
   <si>
     <t>8E</t>
   </si>
@@ -25,55 +34,37 @@
     <t>10E</t>
   </si>
   <si>
+    <t>10Б</t>
+  </si>
+  <si>
     <t>11E</t>
   </si>
   <si>
-    <t>6E</t>
-  </si>
-  <si>
-    <t>7E</t>
-  </si>
-  <si>
     <t>Понедельн.
-22 Янв.</t>
-  </si>
-  <si>
-    <t>Физика (ЮН)</t>
-  </si>
-  <si>
-    <t>Химия (G1234re213)</t>
-  </si>
-  <si>
-    <t>Англ.яз. (Ольга)</t>
-  </si>
-  <si>
-    <t>Химия (Greeeg)</t>
-  </si>
-  <si>
-    <t>География (Гриц)</t>
-  </si>
-  <si>
-    <t>Физика (Гриц)</t>
-  </si>
-  <si>
-    <t>Понедельн.
-23 Янв.</t>
+20 Мар.</t>
+  </si>
+  <si>
+    <t>История (Настя)</t>
   </si>
   <si>
     <t>Вторник
-24 Янв.</t>
+21 Мар.</t>
   </si>
   <si>
     <t>Среда
-25 Янв.</t>
+22 Мар.</t>
   </si>
   <si>
     <t>Четверг
-26 Янв.</t>
+23 Мар.</t>
   </si>
   <si>
     <t>Пяница
-27 Янв.</t>
+24 Мар.</t>
+  </si>
+  <si>
+    <t>Суббота
+25 Мар.</t>
   </si>
 </sst>
 </file>
@@ -103,7 +94,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFFF01"/>
+        <fgColor rgb="00bb7bee"/>
       </patternFill>
     </fill>
     <fill>
@@ -125,8 +116,11 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -435,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,326 +445,267 @@
     <col customWidth="1" max="6" min="6" width="17"/>
     <col customWidth="1" max="7" min="7" width="17"/>
     <col customWidth="1" max="8" min="8" width="17"/>
+    <col customWidth="1" max="9" min="9" width="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:9">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row customHeight="1" ht="18" r="2" spans="1:8">
-      <c r="A2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="n">
+      <c r="I2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="B3" s="3" t="n">
+    </row>
+    <row customHeight="1" ht="25" r="4" spans="1:9">
+      <c r="B4" s="4" t="n">
         <v>2</v>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="4" spans="1:8">
-      <c r="B4" s="3" t="n">
+    <row r="5" spans="1:9">
+      <c r="B5" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="4" t="s">
+    </row>
+    <row r="6" spans="1:9">
+      <c r="B6" s="4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="B7" s="4" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="B8" s="4" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="6" t="n"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="27" r="5" spans="1:8">
-      <c r="B5" s="3" t="n">
+      <c r="B10" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="B11" s="4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="B12" s="4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="B13" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="27" r="6" spans="1:8">
-      <c r="B6" s="3" t="n">
+    </row>
+    <row r="14" spans="1:9">
+      <c r="B14" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="4" t="s">
+    </row>
+    <row r="15" spans="1:9">
+      <c r="B15" s="4" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="6" t="n"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row customHeight="1" ht="22" r="7" spans="1:8">
-      <c r="B7" s="3" t="n">
+      <c r="B17" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="B18" s="4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="B19" s="4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="B20" s="4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="B21" s="4" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="B22" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="H7" s="4" t="s">
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="6" t="n"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="5" t="n"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="2" t="s">
+      <c r="B24" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="B25" s="4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="B26" s="4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="B27" s="4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="B28" s="4" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="B29" s="4" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="6" t="n"/>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="3" t="n">
+      <c r="B31" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row customHeight="1" ht="27" r="10" spans="1:8">
-      <c r="B10" s="3" t="n">
+    <row r="32" spans="1:9">
+      <c r="B32" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="18" r="11" spans="1:8">
-      <c r="B11" s="3" t="n">
+    </row>
+    <row r="33" spans="1:9">
+      <c r="B33" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="27" r="12" spans="1:8">
-      <c r="B12" s="3" t="n">
+    </row>
+    <row r="34" spans="1:9">
+      <c r="B34" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="27" r="13" spans="1:8">
-      <c r="B13" s="3" t="n">
+    </row>
+    <row r="35" spans="1:9">
+      <c r="B35" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="27" r="14" spans="1:8">
-      <c r="B14" s="3" t="n">
+    </row>
+    <row r="36" spans="1:9">
+      <c r="B36" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="5" t="n"/>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="2" t="s">
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="6" t="n"/>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="3" t="n">
+      <c r="B38" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row customHeight="1" ht="23" r="17" spans="1:8">
-      <c r="B17" s="3" t="n">
+    <row r="39" spans="1:9">
+      <c r="B39" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="22" r="18" spans="1:8">
-      <c r="B18" s="3" t="n">
+    </row>
+    <row r="40" spans="1:9">
+      <c r="B40" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="H18" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="B19" s="3" t="n">
+    </row>
+    <row r="41" spans="1:9">
+      <c r="B41" s="4" t="n">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
-      <c r="B20" s="3" t="n">
+    <row r="42" spans="1:9">
+      <c r="B42" s="4" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
-      <c r="B21" s="3" t="n">
+    <row r="43" spans="1:9">
+      <c r="B43" s="4" t="n">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="5" t="n"/>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="B24" s="3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="B25" s="3" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="B26" s="3" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="B27" s="3" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="B28" s="3" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="5" t="n"/>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B30" s="3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="27" r="31" spans="1:8">
-      <c r="B31" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="B32" s="3" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="B33" s="3" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="B34" s="3" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="B35" s="3" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="5" t="n"/>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B37" s="3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="B38" s="3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="B39" s="3" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
-      <c r="B40" s="3" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="B41" s="3" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
-      <c r="B42" s="3" t="n">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A16:A21"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="A22:H22"/>
-    <mergeCell ref="A30:A35"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="A37:A42"/>
-    <mergeCell ref="A36:H36"/>
+  <mergeCells count="12">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="A9:I9"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="A16:I16"/>
+    <mergeCell ref="A17:A22"/>
+    <mergeCell ref="A23:I23"/>
+    <mergeCell ref="A24:A29"/>
+    <mergeCell ref="A30:I30"/>
+    <mergeCell ref="A31:A36"/>
+    <mergeCell ref="A37:I37"/>
+    <mergeCell ref="A38:A43"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>